<commit_message>
Cauldron Room Work + Burndown Update
Textures and some models for the caldruon room added. Thats all I'm doing for now. Might do a little in the evening though I won't push it up till tomorrow.
</commit_message>
<xml_diff>
--- a/Documents/Agile Documents/Burndown Charts/Burndown - Sprint 1.xlsx
+++ b/Documents/Agile Documents/Burndown Charts/Burndown - Sprint 1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\#  Solent Uni Work (2017 - Present Day)\4. Year 2 - 2nd Semester\Software Engineering for Games. Methods and Tools\AE2\SWEG-MT-Project-PT2\Documents\Agile Documents\Burndown Charts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\J\Desktop\SWEG-MT-Project-PT2\Documents\Agile Documents\Burndown Charts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0091739-AE69-4F91-A78C-C2F964D75F0C}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2290F26-6B52-48FE-80A1-C1E948CFB4BC}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="10110" xr2:uid="{F9C6FB3B-61EE-444D-871F-90317262C968}"/>
   </bookViews>
@@ -450,13 +450,13 @@
                   <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>38</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>38</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>38</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1523,7 +1523,7 @@
   <dimension ref="A2:J38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1575,15 +1575,15 @@
       </c>
       <c r="F3" s="2">
         <f>$C3-SUM(C7:E38)</f>
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="G3" s="2">
         <f>$C3-SUM(C7:F38)</f>
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="H3" s="2">
         <f>$C3-SUM(C7:G38)</f>
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
@@ -1725,7 +1725,7 @@
         <v>0</v>
       </c>
       <c r="E9" s="8">
-        <v>0</v>
+        <v>4.5</v>
       </c>
       <c r="F9" s="8">
         <v>0</v>
@@ -1750,7 +1750,7 @@
         <v>0</v>
       </c>
       <c r="E10" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F10" s="8">
         <v>0</v>
@@ -1775,7 +1775,7 @@
         <v>0</v>
       </c>
       <c r="E11" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F11" s="8">
         <v>0</v>
@@ -1800,7 +1800,7 @@
         <v>0</v>
       </c>
       <c r="E12" s="8">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="F12" s="8">
         <v>0</v>
@@ -1875,7 +1875,7 @@
         <v>0</v>
       </c>
       <c r="E15" s="8">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="F15" s="8">
         <v>0</v>
@@ -1900,7 +1900,7 @@
         <v>0</v>
       </c>
       <c r="E16" s="8">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="F16" s="8">
         <v>0</v>

</xml_diff>

<commit_message>
Upper Floor Doors & Sprint #3 Docs
</commit_message>
<xml_diff>
--- a/Documents/Agile Documents/Burndown Charts/Burndown - Sprint 1.xlsx
+++ b/Documents/Agile Documents/Burndown Charts/Burndown - Sprint 1.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
   <si>
     <t>Task</t>
   </si>
@@ -105,6 +105,15 @@
   </si>
   <si>
     <t>Thurs</t>
+  </si>
+  <si>
+    <t>Verlocity</t>
+  </si>
+  <si>
+    <t>Completed</t>
+  </si>
+  <si>
+    <t>y</t>
   </si>
 </sst>
 </file>
@@ -214,7 +223,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -242,6 +251,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1521,10 +1539,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:J38"/>
+  <dimension ref="A2:L38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1659,8 +1677,10 @@
       <c r="G6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
+      <c r="H6" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="I6" s="12"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
@@ -1684,8 +1704,10 @@
       <c r="G7" s="8">
         <v>0</v>
       </c>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
+      <c r="H7" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="I7" s="13"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
@@ -1709,8 +1731,10 @@
       <c r="G8" s="8">
         <v>0</v>
       </c>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
+      <c r="H8" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="I8" s="13"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
@@ -1734,8 +1758,10 @@
       <c r="G9" s="8">
         <v>0.5</v>
       </c>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
+      <c r="H9" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="I9" s="13"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
@@ -1759,8 +1785,10 @@
       <c r="G10" s="8">
         <v>1</v>
       </c>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
+      <c r="H10" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="I10" s="13"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
@@ -1784,8 +1812,8 @@
       <c r="G11" s="8">
         <v>1</v>
       </c>
-      <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="13"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
@@ -1809,8 +1837,8 @@
       <c r="G12" s="8">
         <v>0</v>
       </c>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="13"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
@@ -1834,8 +1862,8 @@
       <c r="G13" s="8">
         <v>0</v>
       </c>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="13"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
@@ -1859,8 +1887,8 @@
       <c r="G14" s="8">
         <v>2</v>
       </c>
-      <c r="H14" s="8"/>
-      <c r="I14" s="8"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="13"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
@@ -1884,8 +1912,8 @@
       <c r="G15" s="8">
         <v>0</v>
       </c>
-      <c r="H15" s="8"/>
-      <c r="I15" s="8"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="13"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
@@ -1909,10 +1937,12 @@
       <c r="G16" s="8">
         <v>0</v>
       </c>
-      <c r="H16" s="8"/>
-      <c r="I16" s="8"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H16" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="I16" s="13"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
       <c r="B17" s="8">
         <v>0</v>
@@ -1932,10 +1962,10 @@
       <c r="G17" s="8">
         <v>0</v>
       </c>
-      <c r="H17" s="8"/>
-      <c r="I17" s="8"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H17" s="13"/>
+      <c r="I17" s="13"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="7"/>
       <c r="B18" s="8">
         <v>0</v>
@@ -1955,10 +1985,10 @@
       <c r="G18" s="8">
         <v>0</v>
       </c>
-      <c r="H18" s="8"/>
-      <c r="I18" s="8"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H18" s="13"/>
+      <c r="I18" s="13"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="7"/>
       <c r="B19" s="8">
         <v>0</v>
@@ -1978,10 +2008,10 @@
       <c r="G19" s="8">
         <v>0</v>
       </c>
-      <c r="H19" s="8"/>
-      <c r="I19" s="8"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H19" s="13"/>
+      <c r="I19" s="13"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
       <c r="B20" s="8">
         <v>0</v>
@@ -2001,10 +2031,10 @@
       <c r="G20" s="8">
         <v>0</v>
       </c>
-      <c r="H20" s="8"/>
-      <c r="I20" s="8"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H20" s="13"/>
+      <c r="I20" s="13"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
       <c r="B21" s="8">
         <v>0</v>
@@ -2024,10 +2054,10 @@
       <c r="G21" s="8">
         <v>0</v>
       </c>
-      <c r="H21" s="8"/>
-      <c r="I21" s="8"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H21" s="13"/>
+      <c r="I21" s="13"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="7"/>
       <c r="B22" s="8">
         <v>0</v>
@@ -2047,10 +2077,10 @@
       <c r="G22" s="8">
         <v>0</v>
       </c>
-      <c r="H22" s="8"/>
-      <c r="I22" s="8"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H22" s="13"/>
+      <c r="I22" s="13"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="7"/>
       <c r="B23" s="8">
         <v>0</v>
@@ -2070,10 +2100,10 @@
       <c r="G23" s="8">
         <v>0</v>
       </c>
-      <c r="H23" s="8"/>
-      <c r="I23" s="8"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H23" s="13"/>
+      <c r="I23" s="13"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="7"/>
       <c r="B24" s="8">
         <v>0</v>
@@ -2093,10 +2123,14 @@
       <c r="G24" s="8">
         <v>0</v>
       </c>
-      <c r="H24" s="8"/>
-      <c r="I24" s="8"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H24" s="13"/>
+      <c r="I24" s="13"/>
+      <c r="K24" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="L24" s="11"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="7"/>
       <c r="B25" s="8">
         <v>0</v>
@@ -2116,10 +2150,15 @@
       <c r="G25" s="8">
         <v>0</v>
       </c>
-      <c r="H25" s="8"/>
-      <c r="I25" s="8"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H25" s="13"/>
+      <c r="I25" s="13"/>
+      <c r="K25" s="11">
+        <f>SUM(B7+B8+B9+B10+B16)</f>
+        <v>19</v>
+      </c>
+      <c r="L25" s="11"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="7"/>
       <c r="B26" s="8">
         <v>0</v>
@@ -2139,10 +2178,10 @@
       <c r="G26" s="8">
         <v>0</v>
       </c>
-      <c r="H26" s="8"/>
-      <c r="I26" s="8"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H26" s="13"/>
+      <c r="I26" s="13"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="7"/>
       <c r="B27" s="8">
         <v>0</v>
@@ -2162,10 +2201,10 @@
       <c r="G27" s="8">
         <v>0</v>
       </c>
-      <c r="H27" s="8"/>
-      <c r="I27" s="8"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H27" s="13"/>
+      <c r="I27" s="13"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="7"/>
       <c r="B28" s="8">
         <v>0</v>
@@ -2185,10 +2224,10 @@
       <c r="G28" s="8">
         <v>0</v>
       </c>
-      <c r="H28" s="8"/>
-      <c r="I28" s="8"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H28" s="13"/>
+      <c r="I28" s="13"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="7"/>
       <c r="B29" s="8">
         <v>0</v>
@@ -2208,10 +2247,10 @@
       <c r="G29" s="8">
         <v>0</v>
       </c>
-      <c r="H29" s="8"/>
-      <c r="I29" s="8"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H29" s="13"/>
+      <c r="I29" s="13"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="7"/>
       <c r="B30" s="8">
         <v>0</v>
@@ -2231,10 +2270,10 @@
       <c r="G30" s="8">
         <v>0</v>
       </c>
-      <c r="H30" s="8"/>
-      <c r="I30" s="8"/>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H30" s="13"/>
+      <c r="I30" s="13"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="7"/>
       <c r="B31" s="8">
         <v>0</v>
@@ -2254,10 +2293,10 @@
       <c r="G31" s="8">
         <v>0</v>
       </c>
-      <c r="H31" s="8"/>
-      <c r="I31" s="8"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H31" s="13"/>
+      <c r="I31" s="13"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="7"/>
       <c r="B32" s="8">
         <v>0</v>
@@ -2277,8 +2316,8 @@
       <c r="G32" s="8">
         <v>0</v>
       </c>
-      <c r="H32" s="8"/>
-      <c r="I32" s="8"/>
+      <c r="H32" s="13"/>
+      <c r="I32" s="13"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="7"/>
@@ -2300,8 +2339,8 @@
       <c r="G33" s="8">
         <v>0</v>
       </c>
-      <c r="H33" s="8"/>
-      <c r="I33" s="8"/>
+      <c r="H33" s="13"/>
+      <c r="I33" s="13"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="7"/>
@@ -2323,8 +2362,8 @@
       <c r="G34" s="8">
         <v>0</v>
       </c>
-      <c r="H34" s="8"/>
-      <c r="I34" s="8"/>
+      <c r="H34" s="13"/>
+      <c r="I34" s="13"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="7"/>
@@ -2346,8 +2385,8 @@
       <c r="G35" s="8">
         <v>0</v>
       </c>
-      <c r="H35" s="8"/>
-      <c r="I35" s="8"/>
+      <c r="H35" s="13"/>
+      <c r="I35" s="13"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="7"/>
@@ -2369,8 +2408,8 @@
       <c r="G36" s="8">
         <v>0</v>
       </c>
-      <c r="H36" s="8"/>
-      <c r="I36" s="8"/>
+      <c r="H36" s="13"/>
+      <c r="I36" s="13"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="7"/>
@@ -2392,8 +2431,8 @@
       <c r="G37" s="8">
         <v>0</v>
       </c>
-      <c r="H37" s="8"/>
-      <c r="I37" s="8"/>
+      <c r="H37" s="13"/>
+      <c r="I37" s="13"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="7"/>
@@ -2415,10 +2454,47 @@
       <c r="G38" s="8">
         <v>0</v>
       </c>
-      <c r="H38" s="8"/>
-      <c r="I38" s="8"/>
+      <c r="H38" s="13"/>
+      <c r="I38" s="13"/>
     </row>
   </sheetData>
+  <mergeCells count="35">
+    <mergeCell ref="H38:I38"/>
+    <mergeCell ref="H32:I32"/>
+    <mergeCell ref="H33:I33"/>
+    <mergeCell ref="H34:I34"/>
+    <mergeCell ref="H35:I35"/>
+    <mergeCell ref="H36:I36"/>
+    <mergeCell ref="H37:I37"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="K24:L24"/>
+    <mergeCell ref="K25:L25"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="H13:I13"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>